<commit_message>
fix carga masiva ubicaciones
</commit_message>
<xml_diff>
--- a/src/assets/files/9.Ubicaciones.xlsx
+++ b/src/assets/files/9.Ubicaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avictoria\Documents\Proyectos\AgendaDigital\ARCHIVOS PRUEBA\oficiales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1A6401-F58C-4DED-93A7-FB3B111BA5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085A0042-3170-423D-AD4E-635298DE1975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="2688" windowWidth="21756" windowHeight="8868" activeTab="2" xr2:uid="{EE8C235F-C2DD-42FA-8519-754DADD1A24F}"/>
+    <workbookView xWindow="1164" yWindow="2280" windowWidth="21756" windowHeight="8868" activeTab="2" xr2:uid="{EE8C235F-C2DD-42FA-8519-754DADD1A24F}"/>
   </bookViews>
   <sheets>
     <sheet name="A_servicios_especialidades" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>CLAVE ESPECIALIDAD</t>
   </si>
@@ -96,13 +96,16 @@
     <t>TIPO</t>
   </si>
   <si>
-    <t>SERVICIO/ESPECIALIDAD</t>
-  </si>
-  <si>
     <t>Trabajo_Social_01</t>
   </si>
   <si>
     <t>Trab_Social_01</t>
+  </si>
+  <si>
+    <t>CLAVE SERVICIO/ESPECIALIDAD</t>
+  </si>
+  <si>
+    <t>CA01</t>
   </si>
 </sst>
 </file>
@@ -592,7 +595,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,21 +617,21 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -661,21 +664,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002047D94B5E73D04A80AA6844A59F543A" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="19f8b377e75dbac3c1f2314aec064948">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f6edc329ff236629c56e3b879b320d0">
     <xsd:element name="properties">
@@ -789,24 +777,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D34C1B82-784D-4D80-A4ED-6D23366ACFE3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253478BC-F8D3-4710-83BA-7E5A9A010CC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CCB55BA9-D7E5-455C-8E1C-C9CE2855CF86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -820,4 +806,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{253478BC-F8D3-4710-83BA-7E5A9A010CC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D34C1B82-784D-4D80-A4ED-6D23366ACFE3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>